<commit_message>
Changed graphs around a bit.
</commit_message>
<xml_diff>
--- a/puzzle1 results.xlsx
+++ b/puzzle1 results.xlsx
@@ -618,7 +618,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -651,7 +651,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6292,11 +6292,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1137662576"/>
-        <c:axId val="1137663120"/>
+        <c:axId val="-2137375856"/>
+        <c:axId val="-2137376400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1137662576"/>
+        <c:axId val="-2137375856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6309,7 +6309,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6342,7 +6342,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6380,7 +6380,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6395,7 +6395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1137663120"/>
+        <c:crossAx val="-2137376400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6404,7 +6404,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1137663120"/>
+        <c:axId val="-2137376400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6431,7 +6431,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6464,7 +6464,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6496,7 +6496,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6511,7 +6511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1137662576"/>
+        <c:crossAx val="-2137375856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6539,7 +6539,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6579,7 +6579,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="2000"/>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -7449,7 +7449,7 @@
   <dimension ref="A1:J328"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AC13" sqref="AC13"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>